<commit_message>
added assignment prep in class
</commit_message>
<xml_diff>
--- a/Assignment/PumpingStationQ.xlsx
+++ b/Assignment/PumpingStationQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Theo/Instituten-Groepen-Overleggen/IHE/git/TransientGroundwaterFlow/Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{759B3075-1921-1E48-9E8E-30AD9AEB01E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5274AACA-51A7-5746-BDEA-D3A5757D9566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="680" windowWidth="27740" windowHeight="17040" xr2:uid="{146C59FE-C1A0-384C-AFDC-FCA354FD9E72}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15540" windowHeight="11540" xr2:uid="{146C59FE-C1A0-384C-AFDC-FCA354FD9E72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,6 +63,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -106,13 +109,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,15 +431,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13F5BEA-D7C4-2C44-A38B-1435256B64ED}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -461,7 +468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <f t="shared" ref="A2:A33" si="0">DATE(D2,C2,1)</f>
         <v>40179</v>
@@ -485,13 +492,14 @@
         <v>750</v>
       </c>
       <c r="G2">
+        <f>F2</f>
         <v>750</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f t="shared" si="0"/>
         <v>40210</v>
@@ -524,7 +532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>40238</v>
@@ -557,7 +565,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>40269</v>
@@ -589,8 +597,9 @@
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>40299</v>
@@ -622,8 +631,9 @@
         <f t="shared" si="6"/>
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>40330</v>
@@ -656,7 +666,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>40360</v>
@@ -688,8 +698,9 @@
         <f t="shared" si="6"/>
         <v>181</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>40391</v>
@@ -722,7 +733,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>40422</v>
@@ -755,7 +766,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>40452</v>
@@ -788,7 +799,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>40483</v>
@@ -821,7 +832,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>40513</v>
@@ -854,7 +865,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>40544</v>
@@ -887,7 +898,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>40575</v>
@@ -920,7 +931,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>40603</v>

</xml_diff>